<commit_message>
Organization of folders and cleaning of code
</commit_message>
<xml_diff>
--- a/lib/assets/inserts.xlsx
+++ b/lib/assets/inserts.xlsx
@@ -960,9 +960,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="13.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1623,15 +1623,15 @@
   </sheetPr>
   <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.3622448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.5357142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.1836734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Rake init and post-search
</commit_message>
<xml_diff>
--- a/lib/assets/inserts.xlsx
+++ b/lib/assets/inserts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="261">
   <si>
     <t xml:space="preserve">Código</t>
   </si>
@@ -798,6 +798,12 @@
   </si>
   <si>
     <t xml:space="preserve">zeca77@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lauro Zacchi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lauroz@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -807,7 +813,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -831,6 +837,87 @@
       <family val="0"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -850,7 +937,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -859,12 +946,54 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -872,8 +1001,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -897,53 +1041,177 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="22">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -954,15 +1222,15 @@
   </sheetPr>
   <dimension ref="A1:B80"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="13.9030612244898"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="32.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="13.9"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1608,7 +1876,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1621,17 +1889,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B57" activeCellId="0" sqref="B57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.1836734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2057,14 +2325,28 @@
       <c r="B53" s="8" t="s">
         <v>258</v>
       </c>
+      <c r="C53" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adição da bibliografia nas fichas 1 e atualização da lista de professores.
</commit_message>
<xml_diff>
--- a/lib/assets/inserts.xlsx
+++ b/lib/assets/inserts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="287">
   <si>
     <t xml:space="preserve">Código</t>
   </si>
@@ -498,7 +498,7 @@
     <t xml:space="preserve">Nome</t>
   </si>
   <si>
-    <t xml:space="preserve">email</t>
+    <t xml:space="preserve">Email</t>
   </si>
   <si>
     <t xml:space="preserve">Abel Soares Siqueira</t>
@@ -687,13 +687,10 @@
     <t xml:space="preserve">alexandrekirilov@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Kally</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x@x1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*</t>
+    <t xml:space="preserve">Kally Chung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chung.kally@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Liliana Madalena Gramani</t>
@@ -792,10 +789,10 @@
     <t xml:space="preserve">saulopo@yahoo.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Stela</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x@x</t>
+    <t xml:space="preserve">Stela Angelozi Leite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stela_angelozi@yahoo.com.br</t>
   </si>
   <si>
     <t xml:space="preserve">Tanise Carnieri Pierin</t>
@@ -895,7 +892,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1000,7 +997,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1010,26 +1007,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Cambria"/>
-      <family val="1"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -1193,7 +1170,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1202,7 +1179,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1210,7 +1187,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1218,23 +1195,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1242,15 +1211,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1349,18 +1322,19 @@
   </sheetPr>
   <dimension ref="A1:B82"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A54" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C72" activeCellId="0" sqref="C72"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C83" activeCellId="0" sqref="C83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="32.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="13.89"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1368,7 +1342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1376,7 +1350,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1384,7 +1358,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -1392,7 +1366,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -1400,7 +1374,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -1408,7 +1382,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
@@ -1416,7 +1390,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
         <v>14</v>
       </c>
@@ -1424,7 +1398,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
         <v>16</v>
       </c>
@@ -1432,7 +1406,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
         <v>18</v>
       </c>
@@ -1440,7 +1414,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
         <v>19</v>
       </c>
@@ -1448,7 +1422,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
         <v>20</v>
       </c>
@@ -1456,7 +1430,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
         <v>22</v>
       </c>
@@ -1464,7 +1438,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
         <v>24</v>
       </c>
@@ -1472,7 +1446,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
         <v>26</v>
       </c>
@@ -1480,7 +1454,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
         <v>28</v>
       </c>
@@ -1488,7 +1462,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
         <v>30</v>
       </c>
@@ -1496,7 +1470,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
         <v>32</v>
       </c>
@@ -1504,7 +1478,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
         <v>34</v>
       </c>
@@ -1512,7 +1486,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="s">
         <v>36</v>
       </c>
@@ -1520,7 +1494,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
         <v>38</v>
       </c>
@@ -1528,7 +1502,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="s">
         <v>40</v>
       </c>
@@ -1536,7 +1510,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
         <v>42</v>
       </c>
@@ -1544,7 +1518,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
         <v>44</v>
       </c>
@@ -1552,7 +1526,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
         <v>46</v>
       </c>
@@ -1560,7 +1534,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
         <v>48</v>
       </c>
@@ -1568,7 +1542,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
         <v>50</v>
       </c>
@@ -1576,7 +1550,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
         <v>52</v>
       </c>
@@ -1584,7 +1558,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
         <v>54</v>
       </c>
@@ -1592,7 +1566,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
         <v>56</v>
       </c>
@@ -1600,7 +1574,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
         <v>58</v>
       </c>
@@ -1608,7 +1582,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="7" t="s">
         <v>60</v>
       </c>
@@ -1616,7 +1590,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="7" t="s">
         <v>62</v>
       </c>
@@ -1624,7 +1598,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="7" t="s">
         <v>64</v>
       </c>
@@ -1632,7 +1606,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
         <v>66</v>
       </c>
@@ -1640,7 +1614,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="7" t="s">
         <v>68</v>
       </c>
@@ -1648,7 +1622,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="s">
         <v>70</v>
       </c>
@@ -1656,7 +1630,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="s">
         <v>72</v>
       </c>
@@ -1664,7 +1638,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="7" t="s">
         <v>74</v>
       </c>
@@ -1672,7 +1646,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="5" t="s">
         <v>76</v>
       </c>
@@ -1680,7 +1654,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="5" t="s">
         <v>78</v>
       </c>
@@ -1688,7 +1662,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="5" t="s">
         <v>80</v>
       </c>
@@ -1696,7 +1670,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="7" t="s">
         <v>82</v>
       </c>
@@ -1704,7 +1678,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="7" t="s">
         <v>84</v>
       </c>
@@ -1712,7 +1686,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="7" t="s">
         <v>86</v>
       </c>
@@ -1720,7 +1694,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="7" t="s">
         <v>88</v>
       </c>
@@ -1728,7 +1702,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="5" t="s">
         <v>90</v>
       </c>
@@ -1736,7 +1710,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="7" t="s">
         <v>92</v>
       </c>
@@ -1744,7 +1718,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="7" t="s">
         <v>93</v>
       </c>
@@ -1752,7 +1726,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="7" t="s">
         <v>95</v>
       </c>
@@ -1760,7 +1734,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="5" t="s">
         <v>97</v>
       </c>
@@ -1768,7 +1742,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="5" t="s">
         <v>99</v>
       </c>
@@ -1776,7 +1750,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="7" t="s">
         <v>101</v>
       </c>
@@ -1784,7 +1758,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="7" t="s">
         <v>103</v>
       </c>
@@ -1792,7 +1766,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="5" t="s">
         <v>105</v>
       </c>
@@ -1800,7 +1774,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="5" t="s">
         <v>107</v>
       </c>
@@ -1808,7 +1782,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="5" t="s">
         <v>109</v>
       </c>
@@ -1816,7 +1790,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="7" t="s">
         <v>111</v>
       </c>
@@ -1824,7 +1798,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="7" t="s">
         <v>113</v>
       </c>
@@ -1832,7 +1806,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="7" t="s">
         <v>115</v>
       </c>
@@ -1840,7 +1814,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="7" t="s">
         <v>116</v>
       </c>
@@ -1848,7 +1822,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="7" t="s">
         <v>118</v>
       </c>
@@ -1856,7 +1830,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="5" t="s">
         <v>119</v>
       </c>
@@ -1864,7 +1838,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="5" t="s">
         <v>121</v>
       </c>
@@ -1872,7 +1846,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="5" t="s">
         <v>123</v>
       </c>
@@ -1880,7 +1854,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="5" t="s">
         <v>125</v>
       </c>
@@ -1888,7 +1862,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="5" t="s">
         <v>127</v>
       </c>
@@ -1896,7 +1870,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="5" t="s">
         <v>129</v>
       </c>
@@ -1904,7 +1878,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="5" t="s">
         <v>131</v>
       </c>
@@ -1912,7 +1886,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="5" t="s">
         <v>133</v>
       </c>
@@ -1920,7 +1894,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="5" t="s">
         <v>135</v>
       </c>
@@ -1928,7 +1902,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="5" t="s">
         <v>137</v>
       </c>
@@ -1936,7 +1910,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="5" t="s">
         <v>138</v>
       </c>
@@ -1944,7 +1918,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="5" t="s">
         <v>140</v>
       </c>
@@ -1952,7 +1926,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="5" t="s">
         <v>142</v>
       </c>
@@ -1960,7 +1934,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="5" t="s">
         <v>144</v>
       </c>
@@ -1968,7 +1942,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="5" t="s">
         <v>146</v>
       </c>
@@ -1976,7 +1950,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="5" t="s">
         <v>148</v>
       </c>
@@ -1984,7 +1958,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="5" t="s">
         <v>150</v>
       </c>
@@ -1992,7 +1966,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="5" t="s">
         <v>152</v>
       </c>
@@ -2000,7 +1974,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="5" t="s">
         <v>153</v>
       </c>
@@ -2008,7 +1982,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="5" t="s">
         <v>155</v>
       </c>
@@ -2032,484 +2006,474 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A55" activeCellId="0" sqref="A55"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="5" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="5" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="5" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="5" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="5" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="5" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="5" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="5" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="5" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="5" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="s">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="5" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="5" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="5" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="5" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="5" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="5" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="5" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="5" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="5" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="5" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="5" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="5" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="5" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="5" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="5" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="5" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="5" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="5" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="5" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="5" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="5" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="8" t="s">
+      <c r="A32" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="5" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="8" t="s">
+      <c r="A33" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="D33" s="0" t="s">
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="5" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="8" t="s">
+      <c r="B34" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="B34" s="8" t="s">
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="5" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="8" t="s">
+      <c r="B35" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="B35" s="8" t="s">
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="5" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="8" t="s">
+      <c r="B36" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="B36" s="8" t="s">
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="5" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="8" t="s">
+      <c r="B37" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B37" s="8" t="s">
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="5" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="8" t="s">
+      <c r="B38" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="B38" s="8" t="s">
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="5" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="8" t="s">
+      <c r="B39" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="B39" s="8" t="s">
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="5" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="8" t="s">
+      <c r="B40" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="B40" s="8" t="s">
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="5" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="8" t="s">
+      <c r="B41" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="B41" s="8" t="s">
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="5" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="8" t="s">
+      <c r="B42" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="B42" s="8" t="s">
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="5" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="8" t="s">
+      <c r="B43" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="B43" s="8" t="s">
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="5" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="8" t="s">
+      <c r="B44" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="B44" s="8" t="s">
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="5" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="8" t="s">
+      <c r="B45" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="B45" s="8" t="s">
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="5" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="8" t="s">
+      <c r="B46" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="B46" s="8" t="s">
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="5" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="8" t="s">
+      <c r="B47" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="B47" s="8" t="s">
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="5" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="8" t="s">
+      <c r="B48" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="B48" s="8" t="s">
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="5" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="8" t="s">
+      <c r="B49" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="B49" s="8" t="s">
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="5" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="8" t="s">
+      <c r="B50" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="B50" s="10" t="s">
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="D50" s="0" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="8" t="s">
+      <c r="B51" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="B51" s="8" t="s">
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="5" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="8" t="s">
+      <c r="B52" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="B52" s="8" t="s">
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="5" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="8" t="s">
+      <c r="B53" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="B53" s="8" t="s">
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="5" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="8" t="s">
+      <c r="B54" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="B54" s="8" t="s">
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="5" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="8" t="s">
+      <c r="B55" s="5" t="s">
         <v>266</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>267</v>
       </c>
       <c r="C55" s="0" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="11" t="s">
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="B56" s="8" t="s">
         <v>268</v>
-      </c>
-      <c r="B56" s="11" t="s">
-        <v>269</v>
       </c>
       <c r="C56" s="0" t="n">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B33" r:id="rId1" display="x@x1"/>
-    <hyperlink ref="B50" r:id="rId2" display="x@x"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2527,202 +2491,202 @@
   </sheetPr>
   <dimension ref="A1:D108"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C65" activeCellId="0" sqref="C65"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="33.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="31.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="11" width="46.12"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="11" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="9" width="33.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="9" width="4.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="9" width="46.12"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="9" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>270</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
+      <c r="C2" s="13" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B3" s="11" t="s">
         <v>271</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="s">
+      <c r="C3" s="12" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B4" s="11" t="s">
         <v>272</v>
       </c>
-      <c r="C3" s="14" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
+      <c r="C4" s="13" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B5" s="11" t="s">
         <v>273</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="s">
+      <c r="C5" s="12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B8" s="11" t="s">
         <v>274</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C8" s="12" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C6" s="14" t="s">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="C10" s="12" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12" t="s">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>275</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12" t="s">
+      <c r="B11" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="13" t="s">
-        <v>276</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>277</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="13" t="s">
+      <c r="B12" s="11" t="s">
         <v>278</v>
       </c>
-      <c r="C11" s="14" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>279</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>240</v>
+      <c r="C12" s="12" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="13" t="s">
-        <v>280</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>246</v>
+      <c r="B13" s="11" t="s">
+        <v>279</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="13" t="s">
-        <v>281</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>234</v>
+      <c r="B14" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="13" t="s">
-        <v>282</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>236</v>
+      <c r="B15" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="13" t="s">
-        <v>270</v>
+      <c r="B16" s="11" t="s">
+        <v>269</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="B17" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C17" s="14" t="s">
+      <c r="B17" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C17" s="12" t="s">
         <v>203</v>
       </c>
     </row>
@@ -2730,21 +2694,21 @@
       <c r="A18" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="13" t="s">
-        <v>272</v>
+      <c r="B18" s="11" t="s">
+        <v>271</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="13" t="s">
-        <v>273</v>
-      </c>
-      <c r="C19" s="14" t="s">
+      <c r="B19" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="C19" s="12" t="s">
         <v>195</v>
       </c>
     </row>
@@ -2752,131 +2716,131 @@
       <c r="A20" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="13" t="s">
-        <v>274</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>246</v>
+      <c r="B20" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="11" t="s">
         <v>270</v>
       </c>
-      <c r="C21" s="14" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="12" t="s">
+      <c r="C22" s="12" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B25" s="11" t="s">
         <v>271</v>
       </c>
-      <c r="C22" s="14" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="12" t="s">
+      <c r="C25" s="12" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="B23" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="B24" s="13" t="s">
+      <c r="B31" s="11" t="s">
         <v>271</v>
       </c>
-      <c r="C24" s="14" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>272</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>273</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>274</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>272</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>272</v>
-      </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="12" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2884,10 +2848,10 @@
       <c r="A32" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="13" t="s">
-        <v>275</v>
-      </c>
-      <c r="C32" s="14" t="s">
+      <c r="B32" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="C32" s="12" t="s">
         <v>163</v>
       </c>
     </row>
@@ -2895,10 +2859,10 @@
       <c r="A33" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B33" s="13" t="s">
-        <v>276</v>
-      </c>
-      <c r="C33" s="14" t="s">
+      <c r="B33" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="C33" s="12" t="s">
         <v>213</v>
       </c>
     </row>
@@ -2906,13 +2870,13 @@
       <c r="A34" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C34" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="D34" s="11" t="n">
+      <c r="B34" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="D34" s="9" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2920,13 +2884,13 @@
       <c r="A35" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="B35" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C35" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="D35" s="11" t="n">
+      <c r="B35" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="D35" s="9" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2934,54 +2898,54 @@
       <c r="A36" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="13" t="s">
+      <c r="B36" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="11" t="s">
         <v>271</v>
       </c>
-      <c r="C36" s="14" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B37" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C37" s="14" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B38" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="C38" s="14" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B39" s="13" t="s">
-        <v>272</v>
-      </c>
-      <c r="C39" s="14" t="s">
+      <c r="C39" s="12" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="12" t="s">
+      <c r="A40" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="B40" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C40" s="14" t="s">
+      <c r="B40" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C40" s="12" t="s">
         <v>221</v>
       </c>
     </row>
@@ -2989,10 +2953,10 @@
       <c r="A41" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B41" s="13" t="s">
-        <v>273</v>
-      </c>
-      <c r="C41" s="14" t="s">
+      <c r="B41" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="C41" s="12" t="s">
         <v>177</v>
       </c>
     </row>
@@ -3000,10 +2964,10 @@
       <c r="A42" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B42" s="13" t="s">
-        <v>274</v>
-      </c>
-      <c r="C42" s="14" t="s">
+      <c r="B42" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="C42" s="12" t="s">
         <v>163</v>
       </c>
     </row>
@@ -3011,10 +2975,10 @@
       <c r="A43" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B43" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C43" s="14" t="s">
+      <c r="B43" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C43" s="12" t="s">
         <v>207</v>
       </c>
     </row>
@@ -3022,21 +2986,21 @@
       <c r="A44" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B44" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C44" s="14" t="s">
-        <v>238</v>
+      <c r="B44" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B45" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C45" s="14" t="s">
+      <c r="B45" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C45" s="12" t="s">
         <v>167</v>
       </c>
     </row>
@@ -3044,13 +3008,13 @@
       <c r="A46" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B46" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C46" s="14" t="s">
-        <v>226</v>
-      </c>
-      <c r="D46" s="11" t="n">
+      <c r="B46" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="D46" s="9" t="n">
         <v>2</v>
       </c>
     </row>
@@ -3058,13 +3022,13 @@
       <c r="A47" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B47" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="C47" s="14" t="s">
-        <v>226</v>
-      </c>
-      <c r="D47" s="11" t="n">
+      <c r="B47" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="D47" s="9" t="n">
         <v>2</v>
       </c>
     </row>
@@ -3072,60 +3036,60 @@
       <c r="A48" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B48" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="C48" s="14" t="s">
-        <v>230</v>
+      <c r="B48" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B49" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C49" s="14" t="s">
+      <c r="B49" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C49" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="D49" s="11" t="s">
-        <v>283</v>
+      <c r="D49" s="9" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B50" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C50" s="14" t="s">
-        <v>264</v>
+      <c r="B50" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B51" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C51" s="14" t="s">
+      <c r="B51" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C51" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="D51" s="11" t="s">
-        <v>283</v>
+      <c r="D51" s="9" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B52" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="C52" s="14" t="s">
+      <c r="B52" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="C52" s="12" t="s">
         <v>219</v>
       </c>
     </row>
@@ -3133,10 +3097,10 @@
       <c r="A53" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B53" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C53" s="14" t="s">
+      <c r="B53" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C53" s="12" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3144,21 +3108,21 @@
       <c r="A54" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B54" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C54" s="14" t="s">
-        <v>248</v>
+      <c r="B54" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B55" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C55" s="14" t="s">
+      <c r="B55" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C55" s="12" t="s">
         <v>211</v>
       </c>
     </row>
@@ -3166,10 +3130,10 @@
       <c r="A56" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="B56" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C56" s="14" t="s">
+      <c r="B56" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C56" s="12" t="s">
         <v>207</v>
       </c>
     </row>
@@ -3177,35 +3141,35 @@
       <c r="A57" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C57" s="14" t="s">
+      <c r="B57" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C57" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="D57" s="11" t="s">
-        <v>283</v>
+      <c r="D57" s="9" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="B58" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="C58" s="14" t="s">
-        <v>234</v>
+      <c r="B58" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="B59" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C59" s="14" t="s">
+      <c r="B59" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C59" s="12" t="s">
         <v>167</v>
       </c>
     </row>
@@ -3213,10 +3177,10 @@
       <c r="A60" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="B60" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C60" s="14" t="s">
+      <c r="B60" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C60" s="12" t="s">
         <v>217</v>
       </c>
     </row>
@@ -3224,10 +3188,10 @@
       <c r="A61" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="B61" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="C61" s="14" t="s">
+      <c r="B61" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="C61" s="12" t="s">
         <v>217</v>
       </c>
     </row>
@@ -3235,10 +3199,10 @@
       <c r="A62" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="B62" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C62" s="14" t="s">
+      <c r="B62" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C62" s="12" t="s">
         <v>189</v>
       </c>
     </row>
@@ -3246,10 +3210,10 @@
       <c r="A63" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="B63" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="C63" s="14" t="s">
+      <c r="B63" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="C63" s="12" t="s">
         <v>205</v>
       </c>
     </row>
@@ -3257,10 +3221,10 @@
       <c r="A64" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="B64" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C64" s="14" t="s">
+      <c r="B64" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C64" s="12" t="s">
         <v>181</v>
       </c>
     </row>
@@ -3268,10 +3232,10 @@
       <c r="A65" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="B65" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="C65" s="14" t="s">
+      <c r="B65" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="C65" s="12" t="s">
         <v>169</v>
       </c>
     </row>
@@ -3279,10 +3243,10 @@
       <c r="A66" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="B66" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C66" s="14" t="s">
+      <c r="B66" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C66" s="12" t="s">
         <v>185</v>
       </c>
     </row>
@@ -3290,10 +3254,10 @@
       <c r="A67" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="B67" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="C67" s="14" t="s">
+      <c r="B67" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="C67" s="12" t="s">
         <v>181</v>
       </c>
     </row>
@@ -3301,10 +3265,10 @@
       <c r="A68" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="B68" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C68" s="14" t="s">
+      <c r="B68" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C68" s="12" t="s">
         <v>177</v>
       </c>
     </row>
@@ -3312,10 +3276,10 @@
       <c r="A69" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="B69" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C69" s="14" t="s">
+      <c r="B69" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C69" s="12" t="s">
         <v>193</v>
       </c>
     </row>
@@ -3323,10 +3287,10 @@
       <c r="A70" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="B70" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="C70" s="14" t="s">
+      <c r="B70" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="C70" s="12" t="s">
         <v>197</v>
       </c>
     </row>
@@ -3334,21 +3298,21 @@
       <c r="A71" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="B71" s="13" t="s">
-        <v>270</v>
+      <c r="B71" s="11" t="s">
+        <v>269</v>
       </c>
       <c r="C71" s="13" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="B72" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="C72" s="14" t="s">
+      <c r="B72" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="C72" s="12" t="s">
         <v>183</v>
       </c>
     </row>
@@ -3356,101 +3320,101 @@
       <c r="A73" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="B73" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C73" s="14" t="s">
-        <v>230</v>
+      <c r="B73" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C73" s="12" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="B74" s="13" t="s">
+      <c r="B74" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C74" s="12" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="B75" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C75" s="12" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="B76" s="11" t="s">
         <v>270</v>
       </c>
-      <c r="C74" s="14" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="B75" s="13" t="s">
+      <c r="C76" s="12" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B77" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C77" s="12" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B78" s="11" t="s">
         <v>270</v>
       </c>
-      <c r="C75" s="14" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="B76" s="13" t="s">
+      <c r="C78" s="12" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B79" s="11" t="s">
         <v>271</v>
       </c>
-      <c r="C76" s="14" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="B77" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C77" s="14" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B78" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="C78" s="14" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B79" s="13" t="s">
-        <v>272</v>
-      </c>
-      <c r="C79" s="14" t="s">
-        <v>256</v>
+      <c r="C79" s="13" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="B80" s="13" t="s">
-        <v>273</v>
-      </c>
-      <c r="C80" s="14" t="s">
+      <c r="B80" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="C80" s="12" t="s">
         <v>191</v>
       </c>
-      <c r="D80" s="11" t="s">
-        <v>283</v>
+      <c r="D80" s="9" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="B81" s="13" t="s">
-        <v>274</v>
-      </c>
-      <c r="C81" s="14" t="s">
+      <c r="B81" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="C81" s="12" t="s">
         <v>191</v>
       </c>
     </row>
@@ -3458,10 +3422,10 @@
       <c r="A82" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="B82" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C82" s="14" t="s">
+      <c r="B82" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C82" s="12" t="s">
         <v>191</v>
       </c>
     </row>
@@ -3469,87 +3433,87 @@
       <c r="A83" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="B83" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C83" s="14" t="s">
-        <v>240</v>
+      <c r="B83" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C83" s="12" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="B84" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C84" s="14" t="s">
-        <v>232</v>
+      <c r="B84" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C84" s="12" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="B85" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="C85" s="14" t="s">
-        <v>232</v>
+      <c r="B85" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="C85" s="12" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="B86" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="C86" s="14" t="s">
-        <v>262</v>
+      <c r="B86" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="C86" s="12" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="B87" s="13" t="s">
-        <v>285</v>
-      </c>
-      <c r="C87" s="14" t="s">
-        <v>262</v>
+      <c r="B87" s="11" t="s">
+        <v>284</v>
+      </c>
+      <c r="C87" s="12" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="B88" s="13" t="s">
-        <v>286</v>
-      </c>
-      <c r="C88" s="14" t="s">
-        <v>254</v>
+      <c r="B88" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="C88" s="12" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="B89" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="C89" s="14" t="s">
-        <v>254</v>
+      <c r="B89" s="11" t="s">
+        <v>286</v>
+      </c>
+      <c r="C89" s="12" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="B90" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C90" s="14" t="s">
+      <c r="B90" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C90" s="12" t="s">
         <v>221</v>
       </c>
     </row>
@@ -3557,10 +3521,10 @@
       <c r="A91" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="B91" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="C91" s="14" t="s">
+      <c r="B91" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="C91" s="12" t="s">
         <v>221</v>
       </c>
     </row>
@@ -3568,10 +3532,10 @@
       <c r="A92" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="B92" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C92" s="14" t="s">
+      <c r="B92" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C92" s="12" t="s">
         <v>165</v>
       </c>
     </row>
@@ -3579,10 +3543,10 @@
       <c r="A93" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="B93" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="C93" s="14" t="s">
+      <c r="B93" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="C93" s="12" t="s">
         <v>165</v>
       </c>
     </row>
@@ -3590,10 +3554,10 @@
       <c r="A94" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="B94" s="13" t="s">
-        <v>272</v>
-      </c>
-      <c r="C94" s="14" t="s">
+      <c r="B94" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="C94" s="12" t="s">
         <v>175</v>
       </c>
     </row>
@@ -3601,10 +3565,10 @@
       <c r="A95" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="B95" s="13" t="s">
-        <v>273</v>
-      </c>
-      <c r="C95" s="14" t="s">
+      <c r="B95" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="C95" s="12" t="s">
         <v>175</v>
       </c>
     </row>
@@ -3612,21 +3576,21 @@
       <c r="A96" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="B96" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C96" s="14" t="s">
-        <v>236</v>
+      <c r="B96" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C96" s="12" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="B97" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C97" s="14" t="s">
+      <c r="B97" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C97" s="12" t="s">
         <v>201</v>
       </c>
     </row>
@@ -3634,10 +3598,10 @@
       <c r="A98" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B98" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C98" s="14" t="s">
+      <c r="B98" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C98" s="12" t="s">
         <v>201</v>
       </c>
     </row>
@@ -3645,10 +3609,10 @@
       <c r="A99" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="B99" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C99" s="14" t="s">
+      <c r="B99" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C99" s="12" t="s">
         <v>195</v>
       </c>
     </row>
@@ -3656,54 +3620,54 @@
       <c r="A100" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="B100" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C100" s="14" t="s">
-        <v>248</v>
+      <c r="B100" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C100" s="12" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="B101" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C101" s="14" t="s">
-        <v>250</v>
+      <c r="B101" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C101" s="12" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="B102" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C102" s="14" t="s">
-        <v>240</v>
+      <c r="B102" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C102" s="12" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="B103" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C103" s="14" t="s">
-        <v>238</v>
+      <c r="B103" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C103" s="12" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="B104" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C104" s="14" t="s">
+      <c r="B104" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C104" s="12" t="s">
         <v>211</v>
       </c>
     </row>
@@ -3711,10 +3675,10 @@
       <c r="A105" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="B105" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C105" s="14" t="s">
+      <c r="B105" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C105" s="12" t="s">
         <v>169</v>
       </c>
     </row>
@@ -3722,10 +3686,10 @@
       <c r="A106" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="B106" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C106" s="14" t="s">
+      <c r="B106" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C106" s="12" t="s">
         <v>213</v>
       </c>
     </row>
@@ -3733,10 +3697,10 @@
       <c r="A107" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="B107" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C107" s="14" t="s">
+      <c r="B107" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C107" s="12" t="s">
         <v>165</v>
       </c>
     </row>
@@ -3744,11 +3708,11 @@
       <c r="A108" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="B108" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C108" s="14" t="s">
-        <v>260</v>
+      <c r="B108" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C108" s="12" t="s">
+        <v>259</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Configuração de envio de email para criação de conta
</commit_message>
<xml_diff>
--- a/lib/assets/inserts.xlsx
+++ b/lib/assets/inserts.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Folha2" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Planilha4" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="291">
   <si>
     <t xml:space="preserve">Código</t>
   </si>
@@ -883,6 +884,18 @@
   </si>
   <si>
     <t xml:space="preserve">N2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">leo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">leonardo.godoy.souza@gmai.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jhonson luiz filipe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">foolemdev@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -2009,7 +2022,7 @@
   <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2491,7 +2504,7 @@
   </sheetPr>
   <dimension ref="A1:D108"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A72" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -3724,4 +3737,52 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A2:B3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.95"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>290</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="leonardo.godoy.souza@gmai.com"/>
+    <hyperlink ref="B3" r:id="rId2" display="foolemdev@gmail.com"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Atualização da lista de professores
</commit_message>
<xml_diff>
--- a/lib/assets/inserts.xlsx
+++ b/lib/assets/inserts.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="293">
   <si>
     <t xml:space="preserve">Código</t>
   </si>
@@ -505,7 +505,7 @@
     <t xml:space="preserve">Abel Soares Siqueira</t>
   </si>
   <si>
-    <t xml:space="preserve">nepper271@gmail.com</t>
+    <t xml:space="preserve">abel.s.siqueira@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Ademir Alves Ribeiro</t>
@@ -724,6 +724,12 @@
     <t xml:space="preserve">maelsachine@gmail.com</t>
   </si>
   <si>
+    <t xml:space="preserve">Marco Aurelio Miranda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">marco.miranda@ufpr.br</t>
+  </si>
+  <si>
     <t xml:space="preserve">Marcelo Muniz Silva Alves </t>
   </si>
   <si>
@@ -778,6 +784,12 @@
     <t xml:space="preserve">ristow@ufpr.br</t>
   </si>
   <si>
+    <t xml:space="preserve">Ricardo Paleari da Silva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ricardopaleari@gmail.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">José João Rossetto</t>
   </si>
   <si>
@@ -790,12 +802,6 @@
     <t xml:space="preserve">saulopo@yahoo.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Stela Angelozi Leite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stela_angelozi@yahoo.com.br</t>
-  </si>
-  <si>
     <t xml:space="preserve">Tanise Carnieri Pierin</t>
   </si>
   <si>
@@ -829,7 +835,7 @@
     <t xml:space="preserve">Lauro Zacchi</t>
   </si>
   <si>
-    <t xml:space="preserve">lauroz@gmail.com</t>
+    <t xml:space="preserve">lauroz@ufpr.br</t>
   </si>
   <si>
     <t xml:space="preserve">A</t>
@@ -889,7 +895,7 @@
     <t xml:space="preserve">leo</t>
   </si>
   <si>
-    <t xml:space="preserve">leonardo.godoy.souza@gmai.com</t>
+    <t xml:space="preserve">leonardo.godoy.souza@gmial.com</t>
   </si>
   <si>
     <t xml:space="preserve">jhonson luiz filipe</t>
@@ -905,7 +911,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="19">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1016,11 +1022,23 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -1183,7 +1201,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1216,11 +1234,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1233,6 +1255,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2019,10 +2045,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:C57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2044,7 +2070,7 @@
       <c r="A2" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="8" t="s">
         <v>160</v>
       </c>
     </row>
@@ -2340,8 +2366,11 @@
       <c r="A39" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="8" t="s">
         <v>234</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2420,7 +2449,7 @@
       <c r="A49" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="8" t="s">
         <v>254</v>
       </c>
     </row>
@@ -2428,7 +2457,7 @@
       <c r="A50" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B50" s="5" t="s">
         <v>256</v>
       </c>
     </row>
@@ -2471,22 +2500,36 @@
       <c r="B55" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="C55" s="0" t="n">
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="C56" s="0" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="8" t="s">
-        <v>267</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="C56" s="0" t="n">
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="C57" s="0" t="n">
         <v>3</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="abel.s.siqueira@gmail.com"/>
+    <hyperlink ref="B39" r:id="rId2" display="marco.miranda@ufpr.br"/>
+    <hyperlink ref="B49" r:id="rId3" display="ricardopaleari@gmail.com"/>
+    <hyperlink ref="B57" r:id="rId4" display="lauroz@ufpr.br"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2504,1228 +2547,1228 @@
   </sheetPr>
   <dimension ref="A1:D108"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A72" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A68" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C79" activeCellId="0" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="9" width="33.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="9" width="4.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="9" width="46.12"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="9" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="33.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="4.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="46.12"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="10" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C1" s="12" t="s">
+      <c r="B1" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>276</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>278</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>279</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>283</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="C29" s="13" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>276</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="D34" s="10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="D35" s="10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="D46" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>271</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="s">
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="D47" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="11" t="s">
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B48" s="12" t="s">
         <v>272</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="11" t="s">
+      <c r="C48" s="13" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C53" s="13" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B54" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C54" s="13" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B55" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C55" s="13" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B56" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C56" s="13" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B57" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C57" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B58" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="C58" s="13" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B59" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C59" s="13" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B60" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C60" s="13" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B61" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="C61" s="13" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B62" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C62" s="13" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B63" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="C63" s="13" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B64" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C64" s="13" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B65" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="C65" s="13" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B66" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C66" s="13" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B67" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="C67" s="13" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B68" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C68" s="13" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B69" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C69" s="13" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B70" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="C70" s="13" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B71" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C71" s="15" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B72" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="C72" s="13" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B73" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C73" s="13" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="B74" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C74" s="13" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B75" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C75" s="13" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B76" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="C76" s="13" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B77" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C77" s="13" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B78" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="C78" s="13" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B79" s="12" t="s">
         <v>273</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="11" t="s">
+      <c r="C79" s="14" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="B80" s="12" t="s">
         <v>274</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C80" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="D80" s="10" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="B81" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="C81" s="13" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="B82" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C82" s="13" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="B83" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C83" s="13" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B84" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C84" s="13" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B85" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="C85" s="13" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B86" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="C86" s="13" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B87" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="C87" s="13" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B88" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="C88" s="13" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B89" s="12" t="s">
+        <v>288</v>
+      </c>
+      <c r="C89" s="13" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B90" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C90" s="13" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B91" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="C91" s="13" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B92" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C92" s="13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B93" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="C93" s="13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B94" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="C94" s="13" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B95" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="C95" s="13" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="B96" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C96" s="13" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>275</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>276</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>277</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>278</v>
-      </c>
-      <c r="C12" s="12" t="s">
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="B97" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C97" s="13" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B98" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C98" s="13" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="B99" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C99" s="13" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="B100" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C100" s="13" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B101" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C101" s="13" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B102" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C102" s="13" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="B103" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C103" s="13" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>279</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>281</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>271</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>272</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>273</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>271</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>272</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>273</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>271</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>271</v>
-      </c>
-      <c r="C31" s="12" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>274</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>275</v>
-      </c>
-      <c r="C33" s="12" t="s">
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="B104" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C104" s="13" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="B105" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C105" s="13" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B106" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C106" s="13" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="D34" s="9" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="D35" s="9" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>271</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="B40" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C40" s="12" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>272</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B42" s="11" t="s">
-        <v>273</v>
-      </c>
-      <c r="C42" s="12" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C43" s="12" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B44" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C44" s="12" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B45" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C45" s="12" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B46" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C46" s="12" t="s">
-        <v>225</v>
-      </c>
-      <c r="D46" s="9" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B47" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="C47" s="12" t="s">
-        <v>225</v>
-      </c>
-      <c r="D47" s="9" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B48" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="C48" s="12" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B49" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C49" s="12" t="s">
-        <v>201</v>
-      </c>
-      <c r="D49" s="9" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B50" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C50" s="12" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B51" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C51" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="D51" s="9" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B52" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="C52" s="12" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="B53" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C53" s="12" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="B54" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C54" s="12" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="B55" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C55" s="12" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="B56" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C56" s="12" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="B57" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C57" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="D57" s="9" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="B58" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="C58" s="12" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="B59" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C59" s="12" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="B60" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C60" s="12" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="B61" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="C61" s="12" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="B62" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C62" s="12" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="B63" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="C63" s="12" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="B64" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C64" s="12" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="B65" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="C65" s="12" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="B66" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C66" s="12" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="B67" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="C67" s="12" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="B68" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C68" s="12" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="B69" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C69" s="12" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="B70" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="C70" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="B71" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C71" s="13" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="B72" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="C72" s="12" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="B73" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C73" s="12" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="B74" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C74" s="12" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="B75" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C75" s="12" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="B76" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="C76" s="12" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B77" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C77" s="12" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="B78" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="C78" s="12" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="B79" s="11" t="s">
-        <v>271</v>
-      </c>
-      <c r="C79" s="13" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="B80" s="11" t="s">
-        <v>272</v>
-      </c>
-      <c r="C80" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="D80" s="9" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="B81" s="11" t="s">
-        <v>273</v>
-      </c>
-      <c r="C81" s="12" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="B82" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C82" s="12" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="B83" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C83" s="12" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="B84" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C84" s="12" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="B85" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="C85" s="12" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="B86" s="11" t="s">
-        <v>283</v>
-      </c>
-      <c r="C86" s="12" t="s">
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="B107" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C107" s="13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="B108" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C108" s="13" t="s">
         <v>261</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="B87" s="11" t="s">
-        <v>284</v>
-      </c>
-      <c r="C87" s="12" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="B88" s="11" t="s">
-        <v>285</v>
-      </c>
-      <c r="C88" s="12" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="B89" s="11" t="s">
-        <v>286</v>
-      </c>
-      <c r="C89" s="12" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="B90" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C90" s="12" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="B91" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="C91" s="12" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="B92" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C92" s="12" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="B93" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="C93" s="12" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="B94" s="11" t="s">
-        <v>271</v>
-      </c>
-      <c r="C94" s="12" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="B95" s="11" t="s">
-        <v>272</v>
-      </c>
-      <c r="C95" s="12" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="B96" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C96" s="12" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="B97" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C97" s="12" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B98" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C98" s="12" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="B99" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C99" s="12" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="B100" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C100" s="12" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="B101" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C101" s="12" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="B102" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C102" s="12" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="B103" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C103" s="12" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="B104" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C104" s="12" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="B105" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C105" s="12" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="B106" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C106" s="12" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="B107" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C107" s="12" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="B108" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C108" s="12" t="s">
-        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -3747,34 +3790,35 @@
   <dimension ref="A2:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.95"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.87"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="leonardo.godoy.souza@gmai.com"/>
+    <hyperlink ref="B2" r:id="rId1" display="leonardo.godoy.souza@gmial.com"/>
     <hyperlink ref="B3" r:id="rId2" display="foolemdev@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Atualização da tabela de horarios e jquery no footer
</commit_message>
<xml_diff>
--- a/lib/assets/inserts.xlsx
+++ b/lib/assets/inserts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="308">
   <si>
     <t xml:space="preserve">Código</t>
   </si>
@@ -847,6 +847,9 @@
     <t xml:space="preserve">A</t>
   </si>
   <si>
+    <t xml:space="preserve">07:30 – 09:30</t>
+  </si>
+  <si>
     <t xml:space="preserve">B</t>
   </si>
   <si>
@@ -862,6 +865,9 @@
     <t xml:space="preserve">F</t>
   </si>
   <si>
+    <t xml:space="preserve">13:30 – 15:30</t>
+  </si>
+  <si>
     <t xml:space="preserve">G</t>
   </si>
   <si>
@@ -871,22 +877,55 @@
     <t xml:space="preserve">I</t>
   </si>
   <si>
+    <t xml:space="preserve">17:30 – 19:30</t>
+  </si>
+  <si>
     <t xml:space="preserve">J</t>
   </si>
   <si>
     <t xml:space="preserve">K</t>
   </si>
   <si>
+    <t xml:space="preserve">19:30 – 21:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21:30 – 23:30</t>
+  </si>
+  <si>
     <t xml:space="preserve">L</t>
   </si>
   <si>
     <t xml:space="preserve">Hn</t>
   </si>
   <si>
-    <t xml:space="preserve">x</t>
+    <t xml:space="preserve">09:30 – 11:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20:30 – 23:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20:30 – 22:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18:30 – 20:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15:30 – 17:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19:00 – 22:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13:30 – 17:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19:30 – 23:30</t>
   </si>
   <si>
     <t xml:space="preserve">M1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07:30 – 11:40</t>
   </si>
   <si>
     <t xml:space="preserve">M2</t>
@@ -914,10 +953,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="HH:MM:SS"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1040,6 +1080,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -1202,7 +1248,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1247,6 +1293,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1261,6 +1311,14 @@
     </xf>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2044,13 +2102,13 @@
   </sheetPr>
   <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B54" activeCellId="0" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.34"/>
   </cols>
@@ -2555,1229 +2613,2423 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D108"/>
+  <dimension ref="A1:I108"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A71" activeCellId="0" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="33.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="9.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="4.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="46.12"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="10" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="3" min="3" style="10" width="21.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="11" width="5.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="13.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="11" width="4.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="10" width="12.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="10" width="4.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="10" width="14.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="10" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C1" s="13" t="s">
+      <c r="A1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>171</v>
       </c>
+      <c r="D1" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="F1" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="D2" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="F2" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="20.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="D3" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="F3" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="12" t="s">
+      <c r="D4" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="F4" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="D5" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="F5" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="D6" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="F6" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" s="13" t="s">
         <v>275</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C7" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="D7" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="F7" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="D8" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="F8" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="D9" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="F9" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>282</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="D10" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="F10" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>283</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="D11" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="F11" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="D12" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="F12" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="D13" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="F13" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="20.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>289</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="D14" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="F14" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>290</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>259</v>
+      </c>
+      <c r="D16" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="F16" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="H16" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="D17" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="F17" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="H17" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>259</v>
+      </c>
+      <c r="D18" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="F18" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="H18" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="D19" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="F19" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="H19" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="D20" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="F20" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="H20" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="20.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="D21" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="F21" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="H21" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="I21" s="10" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="20.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="D22" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="F22" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="H22" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="D23" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="F23" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="H23" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="20.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="D24" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="F24" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="H24" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="I24" s="10" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="D25" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="F25" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="H25" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="I25" s="10" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="D26" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="F26" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="H26" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="I26" s="10" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="D27" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="F27" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="H27" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="I27" s="10" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C28" s="14" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="12" t="s">
+      <c r="D28" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="F28" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="D29" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="F29" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="13" t="s">
         <v>276</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C30" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="D30" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="F30" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="20.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="D31" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="F31" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="H31" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="I31" s="10" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="D32" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="F32" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="H32" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="I32" s="10" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="D33" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="F33" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="D34" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="F34" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="D35" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="F35" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="D36" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="F36" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="20.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="D37" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="F37" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="D38" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="F38" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="D39" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="F39" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="D40" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="F40" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="D41" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="F41" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="G41" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="D42" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="F42" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="D43" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="F43" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="G43" s="10" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="D44" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="F44" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G44" s="10" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="D45" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="F45" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G45" s="10" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="D46" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="F46" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G46" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="H46" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="I46" s="10" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="D47" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E47" s="16" t="s">
+        <v>280</v>
+      </c>
+      <c r="F47" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G47" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="H47" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="I47" s="10" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="20.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="D48" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="F48" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G48" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="H48" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="I48" s="10" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="D49" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="F49" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="G49" s="10" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="D50" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="F50" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G50" s="10" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B51" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C51" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="D51" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E51" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="F51" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="G51" s="10" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B52" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="D52" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="F52" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="G52" s="10" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B53" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="D53" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E53" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="F53" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="G53" s="10" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B54" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="D54" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="F54" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G54" s="10" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B55" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="D55" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E55" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="F55" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="G55" s="10" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="D56" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E56" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="F56" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G56" s="10" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B57" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C57" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="D57" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="F57" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G57" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="H57" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="I57" s="10" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B58" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="C58" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="D58" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="F58" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G58" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="H58" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="I58" s="10" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B59" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C59" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="D59" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E59" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="F59" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="G59" s="10" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B60" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C60" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="D60" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="F60" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G60" s="10" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B61" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="C61" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="D61" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="F61" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G61" s="10" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B62" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C62" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="D62" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="F62" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G62" s="10" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B63" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="C63" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="D63" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="F63" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G63" s="10" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B64" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C64" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="D64" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E64" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="F64" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="G64" s="10" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B65" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="C65" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="D65" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E65" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="F65" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="G65" s="10" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B66" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C66" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="D66" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E66" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="F66" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G66" s="10" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B67" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="C67" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="D67" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E67" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="F67" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G67" s="10" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B68" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C68" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="D68" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="E68" s="10" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B69" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C69" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="D69" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="E69" s="10" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B70" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="C70" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="D70" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="E70" s="10" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B71" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C71" s="15" t="s">
+        <v>267</v>
+      </c>
+      <c r="D71" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E71" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="F71" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G71" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="H71" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="I71" s="10" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B72" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="C72" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="D72" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E72" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="F72" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="G72" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="H72" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="I72" s="10" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B73" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C73" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="D73" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E73" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="F73" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G73" s="10" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="B74" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C74" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="D74" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E74" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="F74" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G74" s="10" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="B75" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C75" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="D75" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E75" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="F75" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="G75" s="10" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="B76" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="C76" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="D76" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E76" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="F76" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="G76" s="10" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="B77" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C77" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="D77" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E77" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="F77" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="G77" s="10" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B78" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="C78" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="D78" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="E78" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="F78" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="G78" s="10" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B79" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="C79" s="15" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="12" t="s">
+      <c r="D79" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="E79" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="F79" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="G79" s="10" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="B80" s="13" t="s">
         <v>277</v>
       </c>
-      <c r="C5" s="13" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="B7" s="12" t="s">
+      <c r="C80" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D80" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E80" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="F80" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="G80" s="10" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="B81" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="C81" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D81" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E81" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="F81" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G81" s="10" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="B82" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C82" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D82" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E82" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="F82" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G82" s="10" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="B83" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C83" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="D83" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E83" s="17" t="s">
+        <v>295</v>
+      </c>
+      <c r="F83" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G83" s="10" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B84" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C84" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="D84" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="E84" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>278</v>
-      </c>
-      <c r="C8" s="13" t="s">
+      <c r="F84" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="G84" s="10" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B85" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="C85" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="D85" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="E85" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="F85" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="G85" s="10" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B86" s="13" t="s">
+        <v>299</v>
+      </c>
+      <c r="C86" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="D86" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E86" s="10" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B87" s="13" t="s">
+        <v>301</v>
+      </c>
+      <c r="C87" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="D87" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="E87" s="10" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B88" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="C88" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="D88" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="E88" s="10" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B89" s="13" t="s">
+        <v>303</v>
+      </c>
+      <c r="C89" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="D89" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E89" s="10" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B90" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C90" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="D90" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="E90" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="F90" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="G90" s="10" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B91" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="C91" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="D91" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E91" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="F91" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G91" s="10" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B92" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C92" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="D92" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E92" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="F92" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G92" s="10" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B93" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="C93" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="D93" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E93" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="F93" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G93" s="10" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B94" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="C94" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="D94" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E94" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="F94" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G94" s="10" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B95" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="C95" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="D95" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E95" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="F95" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G95" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="B96" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C96" s="14" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="B97" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C97" s="14" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B98" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C98" s="14" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="B99" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C99" s="14" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="B100" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C100" s="14" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B101" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C101" s="14" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B102" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C102" s="14" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="B103" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C103" s="14" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>279</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>280</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>282</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>283</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>284</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>285</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>275</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>276</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>277</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>274</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>274</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>275</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>276</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>277</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>274</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>275</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="B31" s="12" t="s">
-        <v>275</v>
-      </c>
-      <c r="C31" s="13" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>278</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>279</v>
-      </c>
-      <c r="C33" s="13" t="s">
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="B104" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C104" s="14" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="B105" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C105" s="14" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B106" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C106" s="14" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B34" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="D34" s="10" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C35" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="D35" s="10" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B36" s="12" t="s">
-        <v>274</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B37" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B38" s="12" t="s">
-        <v>274</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B39" s="12" t="s">
-        <v>275</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B41" s="12" t="s">
-        <v>276</v>
-      </c>
-      <c r="C41" s="13" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B42" s="12" t="s">
-        <v>277</v>
-      </c>
-      <c r="C42" s="13" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B43" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C43" s="13" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C44" s="13" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B45" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C45" s="13" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B46" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C46" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="D46" s="10" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>274</v>
-      </c>
-      <c r="C47" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="D47" s="10" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B48" s="12" t="s">
-        <v>274</v>
-      </c>
-      <c r="C48" s="13" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B49" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C49" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="D49" s="10" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="B50" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C50" s="13" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="B51" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C51" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="D51" s="10" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="B52" s="12" t="s">
-        <v>274</v>
-      </c>
-      <c r="C52" s="13" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="B53" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C53" s="13" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B54" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C54" s="13" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="B55" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C55" s="13" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="B56" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C56" s="13" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="B57" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C57" s="13" t="s">
-        <v>205</v>
-      </c>
-      <c r="D57" s="10" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="B58" s="12" t="s">
-        <v>274</v>
-      </c>
-      <c r="C58" s="13" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="B59" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C59" s="13" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="B60" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C60" s="13" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="B61" s="12" t="s">
-        <v>274</v>
-      </c>
-      <c r="C61" s="13" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="B62" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C62" s="13" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="B63" s="12" t="s">
-        <v>274</v>
-      </c>
-      <c r="C63" s="13" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B64" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C64" s="13" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B65" s="12" t="s">
-        <v>274</v>
-      </c>
-      <c r="C65" s="13" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="B66" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C66" s="13" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="B67" s="12" t="s">
-        <v>274</v>
-      </c>
-      <c r="C67" s="13" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="B68" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C68" s="13" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="B69" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C69" s="13" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="B70" s="12" t="s">
-        <v>274</v>
-      </c>
-      <c r="C70" s="13" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="B71" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C71" s="14" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="B72" s="12" t="s">
-        <v>274</v>
-      </c>
-      <c r="C72" s="13" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="B73" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C73" s="13" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="B74" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C74" s="13" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="B75" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C75" s="13" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="B76" s="12" t="s">
-        <v>274</v>
-      </c>
-      <c r="C76" s="13" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="B77" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C77" s="13" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="B78" s="12" t="s">
-        <v>274</v>
-      </c>
-      <c r="C78" s="13" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="B79" s="12" t="s">
-        <v>275</v>
-      </c>
-      <c r="C79" s="14" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="B80" s="12" t="s">
-        <v>276</v>
-      </c>
-      <c r="C80" s="13" t="s">
-        <v>191</v>
-      </c>
-      <c r="D80" s="10" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="B81" s="12" t="s">
-        <v>277</v>
-      </c>
-      <c r="C81" s="13" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="B82" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C82" s="13" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="B83" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C83" s="13" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="B84" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C84" s="13" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="B85" s="12" t="s">
-        <v>274</v>
-      </c>
-      <c r="C85" s="13" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="B86" s="12" t="s">
-        <v>287</v>
-      </c>
-      <c r="C86" s="13" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="B87" s="12" t="s">
-        <v>288</v>
-      </c>
-      <c r="C87" s="13" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="B88" s="12" t="s">
-        <v>289</v>
-      </c>
-      <c r="C88" s="13" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="B89" s="12" t="s">
-        <v>290</v>
-      </c>
-      <c r="C89" s="13" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="B90" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C90" s="13" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="B91" s="12" t="s">
-        <v>274</v>
-      </c>
-      <c r="C91" s="13" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="B92" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C92" s="13" t="s">
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="B107" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C107" s="14" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="B93" s="12" t="s">
-        <v>274</v>
-      </c>
-      <c r="C93" s="13" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="B94" s="12" t="s">
-        <v>275</v>
-      </c>
-      <c r="C94" s="13" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="B95" s="12" t="s">
-        <v>276</v>
-      </c>
-      <c r="C95" s="13" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="B96" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C96" s="13" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="B97" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C97" s="13" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B98" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C98" s="13" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="B99" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C99" s="13" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="B100" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C100" s="13" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="B101" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C101" s="13" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="B102" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C102" s="13" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="B103" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C103" s="13" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="B104" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C104" s="13" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="B105" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C105" s="13" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="B106" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C106" s="13" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="B107" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C107" s="13" t="s">
-        <v>165</v>
-      </c>
-    </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="14" t="s">
+      <c r="A108" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="B108" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="C108" s="13" t="s">
+      <c r="B108" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C108" s="14" t="s">
         <v>261</v>
       </c>
     </row>
@@ -3812,18 +5064,18 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>291</v>
+        <v>304</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>293</v>
+        <v>306</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>294</v>
+        <v>307</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nova tela de junção de turmas
</commit_message>
<xml_diff>
--- a/lib/assets/inserts.xlsx
+++ b/lib/assets/inserts.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="309">
   <si>
     <t xml:space="preserve">Código</t>
   </si>
@@ -920,6 +920,9 @@
   </si>
   <si>
     <t xml:space="preserve">19:30 – 23:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t xml:space="preserve">M1</t>
@@ -1417,7 +1420,7 @@
   <dimension ref="A1:B82"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C83" activeCellId="0" sqref="C83"/>
+      <selection pane="topLeft" activeCell="C83" activeCellId="1" sqref="D:D C83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2103,7 +2106,7 @@
   <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B54" activeCellId="0" sqref="B54"/>
+      <selection pane="topLeft" activeCell="B54" activeCellId="1" sqref="D:D B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2615,15 +2618,15 @@
   </sheetPr>
   <dimension ref="A1:I108"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A71" activeCellId="0" sqref="A71"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D70" activeCellId="0" sqref="D:D"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="4.17"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="3" min="3" style="10" width="21.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="5.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="16.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="11" width="5.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="13.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="11" width="4.86"/>
@@ -4329,7 +4332,7 @@
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="15" t="s">
-        <v>92</v>
+        <v>299</v>
       </c>
       <c r="B71" s="13" t="s">
         <v>273</v>
@@ -4689,7 +4692,7 @@
         <v>105</v>
       </c>
       <c r="B86" s="13" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C86" s="14" t="s">
         <v>263</v>
@@ -4698,7 +4701,7 @@
         <v>3</v>
       </c>
       <c r="E86" s="10" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4706,7 +4709,7 @@
         <v>105</v>
       </c>
       <c r="B87" s="13" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C87" s="14" t="s">
         <v>263</v>
@@ -4715,7 +4718,7 @@
         <v>5</v>
       </c>
       <c r="E87" s="10" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4723,7 +4726,7 @@
         <v>105</v>
       </c>
       <c r="B88" s="13" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C88" s="14" t="s">
         <v>257</v>
@@ -4740,7 +4743,7 @@
         <v>105</v>
       </c>
       <c r="B89" s="13" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C89" s="14" t="s">
         <v>257</v>
@@ -5052,7 +5055,7 @@
   <dimension ref="A2:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="D:D A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5064,18 +5067,18 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tela de Unir Matérias
</commit_message>
<xml_diff>
--- a/lib/assets/inserts.xlsx
+++ b/lib/assets/inserts.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="308">
   <si>
     <t xml:space="preserve">Código</t>
   </si>
@@ -920,9 +920,6 @@
   </si>
   <si>
     <t xml:space="preserve">19:30 – 23:30</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t xml:space="preserve">M1</t>
@@ -960,7 +957,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="HH:MM:SS"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1083,12 +1080,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -1251,7 +1242,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1314,10 +1305,6 @@
     </xf>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1420,7 +1407,7 @@
   <dimension ref="A1:B82"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C83" activeCellId="1" sqref="D:D C83"/>
+      <selection pane="topLeft" activeCell="C83" activeCellId="0" sqref="C83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2106,7 +2093,7 @@
   <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B54" activeCellId="1" sqref="D:D B54"/>
+      <selection pane="topLeft" activeCell="B54" activeCellId="0" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2618,21 +2605,21 @@
   </sheetPr>
   <dimension ref="A1:I108"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D70" activeCellId="0" sqref="D:D"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C83" activeCellId="0" sqref="C83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="9.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="5.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="16.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="24.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="11" width="5.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="13.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="11" width="4.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="10" width="12.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="10" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="10" width="4.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="10" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="10" width="14.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="10" width="11.52"/>
   </cols>
   <sheetData>
@@ -3785,7 +3772,7 @@
       <c r="D47" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="E47" s="16" t="s">
+      <c r="E47" s="10" t="s">
         <v>280</v>
       </c>
       <c r="F47" s="11" t="n">
@@ -4332,7 +4319,7 @@
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="15" t="s">
-        <v>299</v>
+        <v>92</v>
       </c>
       <c r="B71" s="13" t="s">
         <v>273</v>
@@ -4631,7 +4618,7 @@
       <c r="D83" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="E83" s="17" t="s">
+      <c r="E83" s="16" t="s">
         <v>295</v>
       </c>
       <c r="F83" s="11" t="n">
@@ -4692,7 +4679,7 @@
         <v>105</v>
       </c>
       <c r="B86" s="13" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C86" s="14" t="s">
         <v>263</v>
@@ -4701,7 +4688,7 @@
         <v>3</v>
       </c>
       <c r="E86" s="10" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4709,7 +4696,7 @@
         <v>105</v>
       </c>
       <c r="B87" s="13" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C87" s="14" t="s">
         <v>263</v>
@@ -4718,7 +4705,7 @@
         <v>5</v>
       </c>
       <c r="E87" s="10" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4726,7 +4713,7 @@
         <v>105</v>
       </c>
       <c r="B88" s="13" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C88" s="14" t="s">
         <v>257</v>
@@ -4743,7 +4730,7 @@
         <v>105</v>
       </c>
       <c r="B89" s="13" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C89" s="14" t="s">
         <v>257</v>
@@ -5055,7 +5042,7 @@
   <dimension ref="A2:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="D:D A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5067,18 +5054,18 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>305</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>307</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>